<commit_message>
Update Member Evaluation Template.xlsx
</commit_message>
<xml_diff>
--- a/docs/excel/Member Evaluation Template.xlsx
+++ b/docs/excel/Member Evaluation Template.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/raj/Documents/DurhamCollege/AI/Semester_1/Intro-to-AI-AIDI-1100/Assignments/simple-stock-tracker/docs/excel/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8C214326-C9C3-604B-B661-40911BA80767}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9F79A122-9764-6C4B-81DE-CA34BC994C87}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="17500" xr2:uid="{69A74F39-8759-3A40-B69C-1A8D8C8CC39E}"/>
   </bookViews>
@@ -19,7 +19,6 @@
     <sheet name="Nikolai" sheetId="2" r:id="rId4"/>
     <sheet name="Praharsh" sheetId="6" r:id="rId5"/>
     <sheet name="Priyank" sheetId="5" r:id="rId6"/>
-    <sheet name="Raj" sheetId="7" r:id="rId7"/>
   </sheets>
   <calcPr calcId="181029"/>
   <extLst>
@@ -40,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="128" uniqueCount="33">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="108" uniqueCount="31">
   <si>
     <t>Member name</t>
   </si>
@@ -63,9 +62,6 @@
     <t>Priyankkumar Prakashbhai Patel</t>
   </si>
   <si>
-    <t>Raj Dholakia</t>
-  </si>
-  <si>
     <t>Member Evaluation Summary</t>
   </si>
   <si>
@@ -120,15 +116,9 @@
     <t>Group Number: 7</t>
   </si>
   <si>
-    <t>By: [Your Name]</t>
-  </si>
-  <si>
     <t>Student ID</t>
   </si>
   <si>
-    <t>Student ID: [Your ID]</t>
-  </si>
-  <si>
     <t>Project Specialist</t>
   </si>
   <si>
@@ -138,7 +128,10 @@
     <t>Project BA</t>
   </si>
   <si>
-    <t>Project POC</t>
+    <t>By: Raj Dholakia</t>
+  </si>
+  <si>
+    <t>Student ID: 100813041</t>
   </si>
 </sst>
 </file>
@@ -242,8 +235,9 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="12">
+  <cellXfs count="13">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="1" applyAlignment="1">
@@ -277,85 +271,16 @@
     <cellStyle name="Heading 2" xfId="2" builtinId="17"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="26">
+  <dxfs count="22">
     <dxf>
+      <font>
+        <b/>
+      </font>
       <numFmt numFmtId="0" formatCode="General"/>
     </dxf>
     <dxf>
       <font>
         <b val="0"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <name val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <name val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <name val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <name val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
       </font>
     </dxf>
     <dxf>
@@ -732,10 +657,10 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{2A06A505-2445-9C46-82E6-9410BDB43012}" name="Table1" displayName="Table1" ref="A8:C14">
-  <autoFilter ref="A8:C14" xr:uid="{2A06A505-2445-9C46-82E6-9410BDB43012}"/>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A9:B14">
-    <sortCondition ref="A9:A14"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{2A06A505-2445-9C46-82E6-9410BDB43012}" name="Table1" displayName="Table1" ref="A8:C13">
+  <autoFilter ref="A8:C13" xr:uid="{2A06A505-2445-9C46-82E6-9410BDB43012}"/>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A9:B13">
+    <sortCondition ref="A9:A13"/>
   </sortState>
   <tableColumns count="3">
     <tableColumn id="1" xr3:uid="{FA286119-2F9C-DD47-95F7-7D581209A435}" name="Member name" totalsRowLabel="Total" dataDxfId="1"/>
@@ -752,7 +677,7 @@
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="9" xr:uid="{9A4C5BB7-1798-9445-8CF1-DBC0DD1CA85D}" name="Teamwork10" displayName="Teamwork10" ref="A5:B11" totalsRowCount="1">
   <autoFilter ref="A5:B10" xr:uid="{9A4C5BB7-1798-9445-8CF1-DBC0DD1CA85D}"/>
   <tableColumns count="2">
-    <tableColumn id="1" xr3:uid="{086B85A6-6452-6646-B792-6AF51F7BEAD5}" name="Evaluation Metric" totalsRowLabel="Total" dataDxfId="17" totalsRowDxfId="6"/>
+    <tableColumn id="1" xr3:uid="{086B85A6-6452-6646-B792-6AF51F7BEAD5}" name="Evaluation Metric" totalsRowLabel="Total" dataDxfId="17" totalsRowDxfId="3"/>
     <tableColumn id="2" xr3:uid="{EC8683CE-05BF-134F-BD99-CE57FDD3CF87}" name="Score" totalsRowFunction="sum"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
@@ -763,30 +688,8 @@
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="10" xr:uid="{830415BD-D7ED-6C40-9933-C7CE6A9CD127}" name="Communication11" displayName="Communication11" ref="A14:B20" totalsRowCount="1">
   <autoFilter ref="A14:B19" xr:uid="{830415BD-D7ED-6C40-9933-C7CE6A9CD127}"/>
   <tableColumns count="2">
-    <tableColumn id="1" xr3:uid="{B58E16E1-838E-984A-BE11-B2A007B38D7D}" name="Evaluation Metric" totalsRowLabel="Total" dataDxfId="15" totalsRowDxfId="16"/>
+    <tableColumn id="1" xr3:uid="{B58E16E1-838E-984A-BE11-B2A007B38D7D}" name="Evaluation Metric" totalsRowLabel="Total" dataDxfId="16" totalsRowDxfId="2"/>
     <tableColumn id="2" xr3:uid="{042671AC-E709-0F41-957B-7ED06C41A6D6}" name="Score" totalsRowFunction="sum"/>
-  </tableColumns>
-  <tableStyleInfo name="TableStyleLight2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
-</table>
-</file>
-
-<file path=xl/tables/table12.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="13" xr:uid="{48A4E451-4D60-B64D-BB3B-9B6D88652665}" name="Teamwork14" displayName="Teamwork14" ref="A5:B11" totalsRowCount="1">
-  <autoFilter ref="A5:B10" xr:uid="{48A4E451-4D60-B64D-BB3B-9B6D88652665}"/>
-  <tableColumns count="2">
-    <tableColumn id="1" xr3:uid="{589BF57E-836D-114D-B318-87EF8ADAD178}" name="Evaluation Metric" totalsRowLabel="Total" dataDxfId="10" totalsRowDxfId="11"/>
-    <tableColumn id="2" xr3:uid="{3265DB33-496C-1F47-A869-D114215DEBE4}" name="Score" totalsRowFunction="sum"/>
-  </tableColumns>
-  <tableStyleInfo name="TableStyleLight2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
-</table>
-</file>
-
-<file path=xl/tables/table13.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="14" xr:uid="{C092DB98-C882-744B-A3CC-C8177A7E0FEF}" name="Communication15" displayName="Communication15" ref="A14:B20" totalsRowCount="1">
-  <autoFilter ref="A14:B19" xr:uid="{C092DB98-C882-744B-A3CC-C8177A7E0FEF}"/>
-  <tableColumns count="2">
-    <tableColumn id="1" xr3:uid="{C49581B0-7208-624D-8572-3719C7847774}" name="Evaluation Metric" totalsRowLabel="Total" dataDxfId="9" totalsRowDxfId="7"/>
-    <tableColumn id="2" xr3:uid="{53816605-FDF0-C243-931B-5D27CA62ECEE}" name="Score" totalsRowFunction="sum"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -796,7 +699,7 @@
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{BDA623E4-F3D8-1043-8A84-1020F18542B8}" name="Teamwork" displayName="Teamwork" ref="A5:B11" totalsRowCount="1">
   <autoFilter ref="A5:B10" xr:uid="{BDA623E4-F3D8-1043-8A84-1020F18542B8}"/>
   <tableColumns count="2">
-    <tableColumn id="1" xr3:uid="{3EB8713B-136D-E040-9A9D-762C33BD989C}" name="Evaluation Metric" totalsRowLabel="Total" dataDxfId="8" totalsRowDxfId="3"/>
+    <tableColumn id="1" xr3:uid="{3EB8713B-136D-E040-9A9D-762C33BD989C}" name="Evaluation Metric" totalsRowLabel="Total" dataDxfId="13" totalsRowDxfId="12"/>
     <tableColumn id="2" xr3:uid="{715DEEF0-93C8-3F4F-9888-4410AEE0B0A8}" name="Score" totalsRowFunction="sum"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
@@ -807,7 +710,7 @@
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="4" xr:uid="{77FF3FD0-42BB-BC4B-86CA-D7EF9298FDB8}" name="Communication" displayName="Communication" ref="A14:B20" totalsRowCount="1">
   <autoFilter ref="A14:B19" xr:uid="{77FF3FD0-42BB-BC4B-86CA-D7EF9298FDB8}"/>
   <tableColumns count="2">
-    <tableColumn id="1" xr3:uid="{DACA40F5-8AD0-9F4F-8DBB-1EB62DD52BB1}" name="Evaluation Metric" totalsRowLabel="Total" dataDxfId="25" totalsRowDxfId="2"/>
+    <tableColumn id="1" xr3:uid="{DACA40F5-8AD0-9F4F-8DBB-1EB62DD52BB1}" name="Evaluation Metric" totalsRowLabel="Total" dataDxfId="21" totalsRowDxfId="11"/>
     <tableColumn id="2" xr3:uid="{72A4F924-06E4-0E44-8D52-014624E376B2}" name="Score" totalsRowFunction="sum"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
@@ -818,7 +721,7 @@
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="5" xr:uid="{09347334-2B84-0847-99B5-640F7A3D22C4}" name="Teamwork6" displayName="Teamwork6" ref="A5:B11" totalsRowCount="1">
   <autoFilter ref="A5:B10" xr:uid="{09347334-2B84-0847-99B5-640F7A3D22C4}"/>
   <tableColumns count="2">
-    <tableColumn id="1" xr3:uid="{1E06A0F9-96C2-CA43-B2EA-79BFDE04D3D9}" name="Evaluation Metric" totalsRowLabel="Total" dataDxfId="23" totalsRowDxfId="24"/>
+    <tableColumn id="1" xr3:uid="{1E06A0F9-96C2-CA43-B2EA-79BFDE04D3D9}" name="Evaluation Metric" totalsRowLabel="Total" dataDxfId="20" totalsRowDxfId="10"/>
     <tableColumn id="2" xr3:uid="{ACF89812-9553-7D43-9ED1-17E83B053A6F}" name="Score" totalsRowFunction="sum"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
@@ -829,7 +732,7 @@
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="6" xr:uid="{106D202F-629F-9042-8F7D-BAE0F1E5D4D7}" name="Communication7" displayName="Communication7" ref="A14:B20" totalsRowCount="1">
   <autoFilter ref="A14:B19" xr:uid="{106D202F-629F-9042-8F7D-BAE0F1E5D4D7}"/>
   <tableColumns count="2">
-    <tableColumn id="1" xr3:uid="{B2E5DAD7-08FB-F547-A2EA-C2159C56C580}" name="Evaluation Metric" totalsRowLabel="Total" dataDxfId="21" totalsRowDxfId="22"/>
+    <tableColumn id="1" xr3:uid="{B2E5DAD7-08FB-F547-A2EA-C2159C56C580}" name="Evaluation Metric" totalsRowLabel="Total" dataDxfId="19" totalsRowDxfId="9"/>
     <tableColumn id="2" xr3:uid="{2C501D2D-C30F-EA44-9EBB-6CC2CF44D12C}" name="Score" totalsRowFunction="sum"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
@@ -840,7 +743,7 @@
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="7" xr:uid="{6B362E8C-3CD8-E64C-834F-66DD541C69FD}" name="Teamwork8" displayName="Teamwork8" ref="A5:B11" totalsRowCount="1">
   <autoFilter ref="A5:B10" xr:uid="{6B362E8C-3CD8-E64C-834F-66DD541C69FD}"/>
   <tableColumns count="2">
-    <tableColumn id="1" xr3:uid="{616A7ABE-A517-914E-81DF-64548FAD6888}" name="Evaluation Metric" totalsRowLabel="Total" dataDxfId="20" totalsRowDxfId="4"/>
+    <tableColumn id="1" xr3:uid="{616A7ABE-A517-914E-81DF-64548FAD6888}" name="Evaluation Metric" totalsRowLabel="Total" dataDxfId="18" totalsRowDxfId="8"/>
     <tableColumn id="2" xr3:uid="{A186067A-1A9D-B748-B7C5-2FA1B4CC0E69}" name="Score" totalsRowFunction="sum"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
@@ -851,7 +754,7 @@
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="8" xr:uid="{BEEFECDA-0342-404E-AB65-3954E26B27ED}" name="Communication9" displayName="Communication9" ref="A14:B20" totalsRowCount="1">
   <autoFilter ref="A14:B19" xr:uid="{BEEFECDA-0342-404E-AB65-3954E26B27ED}"/>
   <tableColumns count="2">
-    <tableColumn id="1" xr3:uid="{3C419D53-2E3C-3A44-A9DD-33E78BD494AC}" name="Evaluation Metric" totalsRowLabel="Total" dataDxfId="18" totalsRowDxfId="19"/>
+    <tableColumn id="1" xr3:uid="{3C419D53-2E3C-3A44-A9DD-33E78BD494AC}" name="Evaluation Metric" totalsRowLabel="Total" dataDxfId="7" totalsRowDxfId="6"/>
     <tableColumn id="2" xr3:uid="{F8BBF3A2-5700-6942-9C0E-A35A60F21BAB}" name="Score" totalsRowFunction="sum"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
@@ -862,7 +765,7 @@
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="11" xr:uid="{1B41A5C7-3300-8742-9688-CF76E817D45F}" name="Teamwork12" displayName="Teamwork12" ref="A5:B11" totalsRowCount="1">
   <autoFilter ref="A5:B10" xr:uid="{1B41A5C7-3300-8742-9688-CF76E817D45F}"/>
   <tableColumns count="2">
-    <tableColumn id="1" xr3:uid="{08D5B5FE-F575-C44E-A248-00E79626193B}" name="Evaluation Metric" totalsRowLabel="Total" dataDxfId="14" totalsRowDxfId="5"/>
+    <tableColumn id="1" xr3:uid="{08D5B5FE-F575-C44E-A248-00E79626193B}" name="Evaluation Metric" totalsRowLabel="Total" dataDxfId="15" totalsRowDxfId="5"/>
     <tableColumn id="2" xr3:uid="{DD8E89A3-005C-304A-9C6F-EB00ECA1956A}" name="Score" totalsRowFunction="sum"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
@@ -873,7 +776,7 @@
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="12" xr:uid="{85B822E8-E01C-494C-AE4B-CD6846C26581}" name="Communication13" displayName="Communication13" ref="A14:B20" totalsRowCount="1">
   <autoFilter ref="A14:B19" xr:uid="{85B822E8-E01C-494C-AE4B-CD6846C26581}"/>
   <tableColumns count="2">
-    <tableColumn id="1" xr3:uid="{0509159D-1210-FF4B-9E64-0325CC89FCB3}" name="Evaluation Metric" totalsRowLabel="Total" dataDxfId="12" totalsRowDxfId="13"/>
+    <tableColumn id="1" xr3:uid="{0509159D-1210-FF4B-9E64-0325CC89FCB3}" name="Evaluation Metric" totalsRowLabel="Total" dataDxfId="14" totalsRowDxfId="4"/>
     <tableColumn id="2" xr3:uid="{34B26C3A-768F-2040-82E9-F8D80079F0A7}" name="Score" totalsRowFunction="sum"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
@@ -1177,10 +1080,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CB8943A8-5C14-8C48-90D0-4ACBDB3CC596}">
-  <dimension ref="A1:C14"/>
+  <dimension ref="A1:C13"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="150" workbookViewId="0">
-      <selection activeCell="D23" sqref="D23"/>
+      <selection activeCell="D12" sqref="D12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1191,36 +1094,36 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:3" ht="25" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A1" s="4" t="s">
-        <v>8</v>
-      </c>
-      <c r="B1" s="4"/>
-      <c r="C1" s="4"/>
+      <c r="A1" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="B1" s="5"/>
+      <c r="C1" s="5"/>
     </row>
     <row r="2" spans="1:3" ht="17" thickTop="1" x14ac:dyDescent="0.2"/>
     <row r="3" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A3" s="11" t="s">
-        <v>26</v>
-      </c>
-      <c r="B3" s="9"/>
+      <c r="A3" s="12" t="s">
+        <v>29</v>
+      </c>
+      <c r="B3" s="10"/>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A4" s="11" t="s">
-        <v>28</v>
-      </c>
-      <c r="B4" s="9"/>
+      <c r="A4" s="12" t="s">
+        <v>30</v>
+      </c>
+      <c r="B4" s="10"/>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A5" s="10" t="s">
+      <c r="A5" s="11" t="s">
+        <v>23</v>
+      </c>
+      <c r="B5" s="11"/>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A6" s="9" t="s">
         <v>24</v>
       </c>
-      <c r="B5" s="10"/>
-    </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A6" s="8" t="s">
-        <v>25</v>
-      </c>
-      <c r="B6" s="8"/>
+      <c r="B6" s="9"/>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
@@ -1230,85 +1133,72 @@
         <v>1</v>
       </c>
       <c r="C8" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A9" s="1" t="str">
+      <c r="A9" s="2" t="str">
         <f>Komal!A1</f>
         <v>Komal Sodera</v>
       </c>
-      <c r="B9">
+      <c r="B9" s="1">
         <f>Teamwork[[#Totals],[Score]]+Communication[[#Totals],[Score]]</f>
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="C9">
         <v>100798413</v>
       </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A10" s="1" t="str">
+      <c r="A10" s="2" t="str">
         <f>Mervat!A1</f>
         <v>Mervat Mustafa</v>
       </c>
-      <c r="B10">
+      <c r="B10" s="1">
         <f>Teamwork6[[#Totals],[Score]]+Communication7[[#Totals],[Score]]</f>
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="C10">
         <v>100674685</v>
       </c>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A11" s="1" t="str">
+      <c r="A11" s="2" t="str">
         <f>Nikolai!A1</f>
         <v>Nikolai Melnikov</v>
       </c>
-      <c r="B11">
+      <c r="B11" s="1">
         <f>Teamwork8[[#Totals],[Score]]+Communication9[[#Totals],[Score]]</f>
-        <v>0</v>
+        <v>4.75</v>
       </c>
       <c r="C11">
         <v>100807278</v>
       </c>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A12" s="1" t="str">
+      <c r="A12" s="2" t="str">
         <f>Praharsh!A1</f>
         <v>Praharsh Bhatt</v>
       </c>
-      <c r="B12">
+      <c r="B12" s="1">
         <f>Teamwork12[[#Totals],[Score]]+Communication13[[#Totals],[Score]]</f>
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="C12">
         <v>100830799</v>
       </c>
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A13" s="1" t="str">
+      <c r="A13" s="2" t="str">
         <f>Priyank!A1</f>
         <v>Priyankkumar Prakashbhai Patel</v>
       </c>
-      <c r="B13">
+      <c r="B13" s="1">
         <f>Teamwork10[[#Totals],[Score]]+Communication11[[#Totals],[Score]]</f>
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="C13">
         <v>100638875</v>
-      </c>
-    </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A14" s="1" t="str">
-        <f>Raj!A1</f>
-        <v>Raj Dholakia</v>
-      </c>
-      <c r="B14">
-        <f>Teamwork14[[#Totals],[Score]]+Communication15[[#Totals],[Score]]</f>
-        <v>0</v>
-      </c>
-      <c r="C14">
-        <v>100813041</v>
       </c>
     </row>
   </sheetData>
@@ -1319,7 +1209,7 @@
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <ignoredErrors>
-    <ignoredError sqref="B9:B10 B12:B14" calculatedColumn="1"/>
+    <ignoredError sqref="B9:B10 B12:B13" calculatedColumn="1"/>
   </ignoredErrors>
   <tableParts count="1">
     <tablePart r:id="rId1"/>
@@ -1332,7 +1222,7 @@
   <dimension ref="A1:E20"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="G12" sqref="G12"/>
+      <selection activeCell="B20" sqref="B20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1343,122 +1233,152 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:5" ht="21" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="3" t="s">
+      <c r="A1" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="B1" s="3"/>
+      <c r="B1" s="4"/>
     </row>
     <row r="2" spans="1:5" ht="17" thickTop="1" x14ac:dyDescent="0.2">
-      <c r="A2" s="7" t="s">
-        <v>29</v>
-      </c>
-      <c r="B2" s="7"/>
+      <c r="A2" s="8" t="s">
+        <v>26</v>
+      </c>
+      <c r="B2" s="8"/>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="E3" s="2"/>
+      <c r="E3" s="3"/>
     </row>
     <row r="4" spans="1:5" ht="18" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="6" t="s">
-        <v>14</v>
-      </c>
-      <c r="B4" s="6"/>
-      <c r="E4" s="2"/>
+      <c r="A4" s="7" t="s">
+        <v>13</v>
+      </c>
+      <c r="B4" s="7"/>
+      <c r="E4" s="3"/>
     </row>
     <row r="5" spans="1:5" ht="17" thickTop="1" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
+        <v>14</v>
+      </c>
+      <c r="B5" t="s">
         <v>15</v>
       </c>
-      <c r="B5" t="s">
-        <v>16</v>
-      </c>
-      <c r="E5" s="2"/>
+      <c r="E5" s="3"/>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A6" s="2" t="s">
+      <c r="A6" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="B6">
+        <v>0.5</v>
+      </c>
+      <c r="E6" s="3"/>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A7" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="E6" s="2"/>
-    </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A7" s="2" t="s">
+      <c r="B7">
+        <v>0.5</v>
+      </c>
+      <c r="E7" s="3"/>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A8" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="E7" s="2"/>
-    </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A8" s="2" t="s">
+      <c r="B8">
+        <v>0.5</v>
+      </c>
+      <c r="E8" s="3"/>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A9" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="E8" s="2"/>
-    </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A9" s="2" t="s">
+      <c r="B9">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A10" s="3" t="s">
         <v>12</v>
       </c>
-    </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A10" s="2" t="s">
-        <v>13</v>
+      <c r="B10">
+        <v>0.5</v>
       </c>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A11" s="2" t="s">
-        <v>23</v>
+      <c r="A11" s="3" t="s">
+        <v>22</v>
       </c>
       <c r="B11">
         <f>SUBTOTAL(109,Teamwork[Score])</f>
-        <v>0</v>
+        <v>2.5</v>
       </c>
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A12" s="5"/>
+      <c r="A12" s="6"/>
     </row>
     <row r="13" spans="1:5" ht="18" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A13" s="6" t="s">
-        <v>22</v>
-      </c>
-      <c r="B13" s="6"/>
+      <c r="A13" s="7" t="s">
+        <v>21</v>
+      </c>
+      <c r="B13" s="7"/>
     </row>
     <row r="14" spans="1:5" ht="17" thickTop="1" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
+        <v>14</v>
+      </c>
+      <c r="B14" t="s">
         <v>15</v>
       </c>
-      <c r="B14" t="s">
+    </row>
+    <row r="15" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A15" s="3" t="s">
         <v>16</v>
       </c>
-    </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A15" s="2" t="s">
+      <c r="B15">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A16" s="3" t="s">
         <v>17</v>
       </c>
-    </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A16" s="2" t="s">
+      <c r="B16">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="17" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A17" s="3" t="s">
         <v>18</v>
       </c>
-    </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A17" s="2" t="s">
+      <c r="B17">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="18" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A18" s="3" t="s">
         <v>19</v>
       </c>
-    </row>
-    <row r="18" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A18" s="2" t="s">
+      <c r="B18">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="19" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A19" s="3" t="s">
         <v>20</v>
       </c>
-    </row>
-    <row r="19" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A19" s="2" t="s">
-        <v>21</v>
+      <c r="B19">
+        <v>0.5</v>
       </c>
     </row>
     <row r="20" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A20" s="2" t="s">
-        <v>23</v>
+      <c r="A20" s="3" t="s">
+        <v>22</v>
       </c>
       <c r="B20">
         <f>SUBTOTAL(109,Communication[Score])</f>
-        <v>0</v>
+        <v>2.5</v>
       </c>
     </row>
   </sheetData>
@@ -1468,7 +1388,7 @@
     <mergeCell ref="A4:B4"/>
     <mergeCell ref="A2:B2"/>
   </mergeCells>
-  <dataValidations disablePrompts="1" count="1">
+  <dataValidations count="1">
     <dataValidation type="decimal" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B6:B10 B15" xr:uid="{E692A9C2-A741-7C42-8455-D6362085B1D9}">
       <formula1>0</formula1>
       <formula2>0.5</formula2>
@@ -1487,7 +1407,7 @@
   <dimension ref="A1:B20"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2:B2"/>
+      <selection activeCell="B20" sqref="B20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1497,114 +1417,144 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:2" ht="21" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="3" t="s">
+      <c r="A1" s="4" t="s">
         <v>4</v>
       </c>
-      <c r="B1" s="3"/>
+      <c r="B1" s="4"/>
     </row>
     <row r="2" spans="1:2" ht="17" thickTop="1" x14ac:dyDescent="0.2">
-      <c r="A2" s="7" t="s">
-        <v>29</v>
-      </c>
-      <c r="B2" s="7"/>
+      <c r="A2" s="8" t="s">
+        <v>26</v>
+      </c>
+      <c r="B2" s="8"/>
     </row>
     <row r="4" spans="1:2" ht="18" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="6" t="s">
-        <v>14</v>
-      </c>
-      <c r="B4" s="6"/>
+      <c r="A4" s="7" t="s">
+        <v>13</v>
+      </c>
+      <c r="B4" s="7"/>
     </row>
     <row r="5" spans="1:2" ht="17" thickTop="1" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
+        <v>14</v>
+      </c>
+      <c r="B5" t="s">
         <v>15</v>
       </c>
-      <c r="B5" t="s">
-        <v>16</v>
-      </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A6" s="2" t="s">
+      <c r="A6" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="B6">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A7" s="3" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A7" s="2" t="s">
+      <c r="B7">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A8" s="3" t="s">
         <v>10</v>
       </c>
-    </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A8" s="2" t="s">
+      <c r="B8">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A9" s="3" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A9" s="2" t="s">
+      <c r="B9">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A10" s="3" t="s">
         <v>12</v>
       </c>
-    </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A10" s="2" t="s">
-        <v>13</v>
+      <c r="B10">
+        <v>0.5</v>
       </c>
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A11" s="2" t="s">
-        <v>23</v>
+      <c r="A11" s="3" t="s">
+        <v>22</v>
       </c>
       <c r="B11">
         <f>SUBTOTAL(109,Teamwork6[Score])</f>
-        <v>0</v>
+        <v>2.5</v>
       </c>
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A12" s="5"/>
+      <c r="A12" s="6"/>
     </row>
     <row r="13" spans="1:2" ht="18" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A13" s="6" t="s">
-        <v>22</v>
-      </c>
-      <c r="B13" s="6"/>
+      <c r="A13" s="7" t="s">
+        <v>21</v>
+      </c>
+      <c r="B13" s="7"/>
     </row>
     <row r="14" spans="1:2" ht="17" thickTop="1" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
+        <v>14</v>
+      </c>
+      <c r="B14" t="s">
         <v>15</v>
       </c>
-      <c r="B14" t="s">
+    </row>
+    <row r="15" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A15" s="3" t="s">
         <v>16</v>
       </c>
-    </row>
-    <row r="15" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A15" s="2" t="s">
+      <c r="B15">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="16" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A16" s="3" t="s">
         <v>17</v>
       </c>
-    </row>
-    <row r="16" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A16" s="2" t="s">
+      <c r="B16">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="17" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A17" s="3" t="s">
         <v>18</v>
       </c>
-    </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A17" s="2" t="s">
+      <c r="B17">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="18" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A18" s="3" t="s">
         <v>19</v>
       </c>
-    </row>
-    <row r="18" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A18" s="2" t="s">
+      <c r="B18">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="19" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A19" s="3" t="s">
         <v>20</v>
       </c>
-    </row>
-    <row r="19" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A19" s="2" t="s">
-        <v>21</v>
+      <c r="B19">
+        <v>0.5</v>
       </c>
     </row>
     <row r="20" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A20" s="2" t="s">
-        <v>23</v>
+      <c r="A20" s="3" t="s">
+        <v>22</v>
       </c>
       <c r="B20">
         <f>SUBTOTAL(109,Communication7[Score])</f>
-        <v>0</v>
+        <v>2.5</v>
       </c>
     </row>
   </sheetData>
@@ -1633,7 +1583,7 @@
   <dimension ref="A1:B20"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A3" sqref="A3"/>
+      <selection activeCell="B20" sqref="B20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1643,114 +1593,144 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:2" ht="21" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="3" t="s">
+      <c r="A1" s="4" t="s">
         <v>2</v>
       </c>
-      <c r="B1" s="3"/>
+      <c r="B1" s="4"/>
     </row>
     <row r="2" spans="1:2" ht="17" thickTop="1" x14ac:dyDescent="0.2">
-      <c r="A2" s="7" t="s">
-        <v>30</v>
-      </c>
-      <c r="B2" s="7"/>
+      <c r="A2" s="8" t="s">
+        <v>27</v>
+      </c>
+      <c r="B2" s="8"/>
     </row>
     <row r="4" spans="1:2" ht="18" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="6" t="s">
-        <v>14</v>
-      </c>
-      <c r="B4" s="6"/>
+      <c r="A4" s="7" t="s">
+        <v>13</v>
+      </c>
+      <c r="B4" s="7"/>
     </row>
     <row r="5" spans="1:2" ht="17" thickTop="1" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
+        <v>14</v>
+      </c>
+      <c r="B5" t="s">
         <v>15</v>
       </c>
-      <c r="B5" t="s">
-        <v>16</v>
-      </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A6" s="2" t="s">
+      <c r="A6" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="B6">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A7" s="3" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A7" s="2" t="s">
+      <c r="B7">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A8" s="3" t="s">
         <v>10</v>
       </c>
-    </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A8" s="2" t="s">
+      <c r="B8">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A9" s="3" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A9" s="2" t="s">
+      <c r="B9">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A10" s="3" t="s">
         <v>12</v>
       </c>
-    </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A10" s="2" t="s">
-        <v>13</v>
+      <c r="B10">
+        <v>0.5</v>
       </c>
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A11" s="2" t="s">
-        <v>23</v>
+      <c r="A11" s="3" t="s">
+        <v>22</v>
       </c>
       <c r="B11">
         <f>SUBTOTAL(109,Teamwork8[Score])</f>
-        <v>0</v>
+        <v>2.5</v>
       </c>
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A12" s="5"/>
+      <c r="A12" s="6"/>
     </row>
     <row r="13" spans="1:2" ht="18" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A13" s="6" t="s">
-        <v>22</v>
-      </c>
-      <c r="B13" s="6"/>
+      <c r="A13" s="7" t="s">
+        <v>21</v>
+      </c>
+      <c r="B13" s="7"/>
     </row>
     <row r="14" spans="1:2" ht="17" thickTop="1" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
+        <v>14</v>
+      </c>
+      <c r="B14" t="s">
         <v>15</v>
       </c>
-      <c r="B14" t="s">
+    </row>
+    <row r="15" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A15" s="3" t="s">
         <v>16</v>
       </c>
-    </row>
-    <row r="15" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A15" s="2" t="s">
+      <c r="B15">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="16" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A16" s="3" t="s">
         <v>17</v>
       </c>
-    </row>
-    <row r="16" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A16" s="2" t="s">
+      <c r="B16">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="17" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A17" s="3" t="s">
         <v>18</v>
       </c>
-    </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A17" s="2" t="s">
+      <c r="B17">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="18" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A18" s="3" t="s">
         <v>19</v>
       </c>
-    </row>
-    <row r="18" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A18" s="2" t="s">
+      <c r="B18">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="19" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A19" s="3" t="s">
         <v>20</v>
       </c>
-    </row>
-    <row r="19" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A19" s="2" t="s">
-        <v>21</v>
+      <c r="B19">
+        <v>0.25</v>
       </c>
     </row>
     <row r="20" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A20" s="2" t="s">
-        <v>23</v>
+      <c r="A20" s="3" t="s">
+        <v>22</v>
       </c>
       <c r="B20">
         <f>SUBTOTAL(109,Communication9[Score])</f>
-        <v>0</v>
+        <v>2.25</v>
       </c>
     </row>
   </sheetData>
@@ -1761,7 +1741,7 @@
     <mergeCell ref="A2:B2"/>
   </mergeCells>
   <dataValidations count="1">
-    <dataValidation type="decimal" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B6 B15" xr:uid="{51F957F3-6D82-104E-886A-FA3F55541830}">
+    <dataValidation type="decimal" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B6 B15:B19" xr:uid="{51F957F3-6D82-104E-886A-FA3F55541830}">
       <formula1>0</formula1>
       <formula2>0.5</formula2>
     </dataValidation>
@@ -1779,7 +1759,7 @@
   <dimension ref="A1:B20"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D30" sqref="D30"/>
+      <selection activeCell="F23" sqref="F23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1789,114 +1769,144 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:2" ht="21" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="3" t="s">
+      <c r="A1" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="B1" s="3"/>
+      <c r="B1" s="4"/>
     </row>
     <row r="2" spans="1:2" ht="17" thickTop="1" x14ac:dyDescent="0.2">
-      <c r="A2" s="7" t="s">
-        <v>30</v>
-      </c>
-      <c r="B2" s="7"/>
+      <c r="A2" s="8" t="s">
+        <v>27</v>
+      </c>
+      <c r="B2" s="8"/>
     </row>
     <row r="4" spans="1:2" ht="18" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="6" t="s">
-        <v>14</v>
-      </c>
-      <c r="B4" s="6"/>
+      <c r="A4" s="7" t="s">
+        <v>13</v>
+      </c>
+      <c r="B4" s="7"/>
     </row>
     <row r="5" spans="1:2" ht="17" thickTop="1" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
+        <v>14</v>
+      </c>
+      <c r="B5" t="s">
         <v>15</v>
       </c>
-      <c r="B5" t="s">
-        <v>16</v>
-      </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A6" s="2" t="s">
+      <c r="A6" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="B6">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A7" s="3" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A7" s="2" t="s">
+      <c r="B7">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A8" s="3" t="s">
         <v>10</v>
       </c>
-    </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A8" s="2" t="s">
+      <c r="B8">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A9" s="3" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A9" s="2" t="s">
+      <c r="B9">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A10" s="3" t="s">
         <v>12</v>
       </c>
-    </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A10" s="2" t="s">
-        <v>13</v>
+      <c r="B10">
+        <v>0.5</v>
       </c>
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A11" s="2" t="s">
-        <v>23</v>
+      <c r="A11" s="3" t="s">
+        <v>22</v>
       </c>
       <c r="B11">
         <f>SUBTOTAL(109,Teamwork12[Score])</f>
-        <v>0</v>
+        <v>2.5</v>
       </c>
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A12" s="5"/>
+      <c r="A12" s="6"/>
     </row>
     <row r="13" spans="1:2" ht="18" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A13" s="6" t="s">
-        <v>22</v>
-      </c>
-      <c r="B13" s="6"/>
+      <c r="A13" s="7" t="s">
+        <v>21</v>
+      </c>
+      <c r="B13" s="7"/>
     </row>
     <row r="14" spans="1:2" ht="17" thickTop="1" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
+        <v>14</v>
+      </c>
+      <c r="B14" t="s">
         <v>15</v>
       </c>
-      <c r="B14" t="s">
+    </row>
+    <row r="15" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A15" s="3" t="s">
         <v>16</v>
       </c>
-    </row>
-    <row r="15" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A15" s="2" t="s">
+      <c r="B15">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="16" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A16" s="3" t="s">
         <v>17</v>
       </c>
-    </row>
-    <row r="16" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A16" s="2" t="s">
+      <c r="B16">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="17" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A17" s="3" t="s">
         <v>18</v>
       </c>
-    </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A17" s="2" t="s">
+      <c r="B17">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="18" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A18" s="3" t="s">
         <v>19</v>
       </c>
-    </row>
-    <row r="18" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A18" s="2" t="s">
+      <c r="B18">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="19" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A19" s="3" t="s">
         <v>20</v>
       </c>
-    </row>
-    <row r="19" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A19" s="2" t="s">
-        <v>21</v>
+      <c r="B19">
+        <v>0.5</v>
       </c>
     </row>
     <row r="20" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A20" s="2" t="s">
-        <v>23</v>
+      <c r="A20" s="3" t="s">
+        <v>22</v>
       </c>
       <c r="B20">
         <f>SUBTOTAL(109,Communication13[Score])</f>
-        <v>0</v>
+        <v>2.5</v>
       </c>
     </row>
   </sheetData>
@@ -1907,7 +1917,7 @@
     <mergeCell ref="A2:B2"/>
   </mergeCells>
   <dataValidations count="1">
-    <dataValidation type="decimal" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B6 B15" xr:uid="{988930B1-D4DB-C847-AA57-58631C314076}">
+    <dataValidation type="decimal" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B6:B10 B15:B19" xr:uid="{988930B1-D4DB-C847-AA57-58631C314076}">
       <formula1>0</formula1>
       <formula2>0.5</formula2>
     </dataValidation>
@@ -1925,7 +1935,7 @@
   <dimension ref="A1:B20"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="F13" sqref="F13"/>
+      <selection activeCell="B15" sqref="B15:B19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1935,114 +1945,144 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:2" ht="21" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="3" t="s">
+      <c r="A1" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="B1" s="3"/>
+      <c r="B1" s="4"/>
     </row>
     <row r="2" spans="1:2" ht="17" thickTop="1" x14ac:dyDescent="0.2">
-      <c r="A2" s="7" t="s">
-        <v>31</v>
-      </c>
-      <c r="B2" s="7"/>
+      <c r="A2" s="8" t="s">
+        <v>28</v>
+      </c>
+      <c r="B2" s="8"/>
     </row>
     <row r="4" spans="1:2" ht="18" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="6" t="s">
-        <v>14</v>
-      </c>
-      <c r="B4" s="6"/>
+      <c r="A4" s="7" t="s">
+        <v>13</v>
+      </c>
+      <c r="B4" s="7"/>
     </row>
     <row r="5" spans="1:2" ht="17" thickTop="1" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
+        <v>14</v>
+      </c>
+      <c r="B5" t="s">
         <v>15</v>
       </c>
-      <c r="B5" t="s">
-        <v>16</v>
-      </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A6" s="2" t="s">
+      <c r="A6" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="B6">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A7" s="3" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A7" s="2" t="s">
+      <c r="B7">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A8" s="3" t="s">
         <v>10</v>
       </c>
-    </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A8" s="2" t="s">
+      <c r="B8">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A9" s="3" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A9" s="2" t="s">
+      <c r="B9">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A10" s="3" t="s">
         <v>12</v>
       </c>
-    </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A10" s="2" t="s">
-        <v>13</v>
+      <c r="B10">
+        <v>0.5</v>
       </c>
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A11" s="2" t="s">
-        <v>23</v>
+      <c r="A11" s="3" t="s">
+        <v>22</v>
       </c>
       <c r="B11">
         <f>SUBTOTAL(109,Teamwork10[Score])</f>
-        <v>0</v>
+        <v>2.5</v>
       </c>
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A12" s="5"/>
+      <c r="A12" s="6"/>
     </row>
     <row r="13" spans="1:2" ht="18" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A13" s="6" t="s">
-        <v>22</v>
-      </c>
-      <c r="B13" s="6"/>
+      <c r="A13" s="7" t="s">
+        <v>21</v>
+      </c>
+      <c r="B13" s="7"/>
     </row>
     <row r="14" spans="1:2" ht="17" thickTop="1" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
+        <v>14</v>
+      </c>
+      <c r="B14" t="s">
         <v>15</v>
       </c>
-      <c r="B14" t="s">
+    </row>
+    <row r="15" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A15" s="3" t="s">
         <v>16</v>
       </c>
-    </row>
-    <row r="15" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A15" s="2" t="s">
+      <c r="B15">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="16" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A16" s="3" t="s">
         <v>17</v>
       </c>
-    </row>
-    <row r="16" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A16" s="2" t="s">
+      <c r="B16">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="17" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A17" s="3" t="s">
         <v>18</v>
       </c>
-    </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A17" s="2" t="s">
+      <c r="B17">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="18" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A18" s="3" t="s">
         <v>19</v>
       </c>
-    </row>
-    <row r="18" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A18" s="2" t="s">
+      <c r="B18">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="19" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A19" s="3" t="s">
         <v>20</v>
       </c>
-    </row>
-    <row r="19" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A19" s="2" t="s">
-        <v>21</v>
+      <c r="B19">
+        <v>0.5</v>
       </c>
     </row>
     <row r="20" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A20" s="2" t="s">
-        <v>23</v>
+      <c r="A20" s="3" t="s">
+        <v>22</v>
       </c>
       <c r="B20">
         <f>SUBTOTAL(109,Communication11[Score])</f>
-        <v>0</v>
+        <v>2.5</v>
       </c>
     </row>
   </sheetData>
@@ -2053,153 +2093,7 @@
     <mergeCell ref="A2:B2"/>
   </mergeCells>
   <dataValidations count="1">
-    <dataValidation type="decimal" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B6 B15" xr:uid="{97351E64-C073-8647-813E-E51CCDFE1894}">
-      <formula1>0</formula1>
-      <formula2>0.5</formula2>
-    </dataValidation>
-  </dataValidations>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <tableParts count="2">
-    <tablePart r:id="rId1"/>
-    <tablePart r:id="rId2"/>
-  </tableParts>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5CCC32C2-01BA-5646-8A5F-E5F2C40AB51F}">
-  <dimension ref="A1:B20"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="F18" sqref="F18"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
-  <cols>
-    <col min="1" max="1" width="50.1640625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="8.1640625" bestFit="1" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:2" ht="21" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="3" t="s">
-        <v>7</v>
-      </c>
-      <c r="B1" s="3"/>
-    </row>
-    <row r="2" spans="1:2" ht="17" thickTop="1" x14ac:dyDescent="0.2">
-      <c r="A2" s="7" t="s">
-        <v>32</v>
-      </c>
-      <c r="B2" s="7"/>
-    </row>
-    <row r="4" spans="1:2" ht="18" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="6" t="s">
-        <v>14</v>
-      </c>
-      <c r="B4" s="6"/>
-    </row>
-    <row r="5" spans="1:2" ht="17" thickTop="1" x14ac:dyDescent="0.2">
-      <c r="A5" t="s">
-        <v>15</v>
-      </c>
-      <c r="B5" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A6" s="2" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A7" s="2" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A8" s="2" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A9" s="2" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A10" s="2" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A11" s="2" t="s">
-        <v>23</v>
-      </c>
-      <c r="B11">
-        <f>SUBTOTAL(109,Teamwork14[Score])</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A12" s="5"/>
-    </row>
-    <row r="13" spans="1:2" ht="18" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A13" s="6" t="s">
-        <v>22</v>
-      </c>
-      <c r="B13" s="6"/>
-    </row>
-    <row r="14" spans="1:2" ht="17" thickTop="1" x14ac:dyDescent="0.2">
-      <c r="A14" t="s">
-        <v>15</v>
-      </c>
-      <c r="B14" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="15" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A15" s="2" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="16" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A16" s="2" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A17" s="2" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="18" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A18" s="2" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="19" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A19" s="2" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="20" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A20" s="2" t="s">
-        <v>23</v>
-      </c>
-      <c r="B20">
-        <f>SUBTOTAL(109,Communication15[Score])</f>
-        <v>0</v>
-      </c>
-    </row>
-  </sheetData>
-  <mergeCells count="4">
-    <mergeCell ref="A1:B1"/>
-    <mergeCell ref="A4:B4"/>
-    <mergeCell ref="A13:B13"/>
-    <mergeCell ref="A2:B2"/>
-  </mergeCells>
-  <dataValidations count="1">
-    <dataValidation type="decimal" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B6 B15" xr:uid="{DE2583F4-9357-9A48-B5AC-499593A014FF}">
+    <dataValidation type="decimal" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B6:B10 B15:B19" xr:uid="{97351E64-C073-8647-813E-E51CCDFE1894}">
       <formula1>0</formula1>
       <formula2>0.5</formula2>
     </dataValidation>

</xml_diff>